<commit_message>
Evolutions des programmes .ino Présentation pour la journée du 5 mai
</commit_message>
<xml_diff>
--- a/ESP8266 Mini/Table motorisation.xlsx
+++ b/ESP8266 Mini/Table motorisation.xlsx
@@ -24,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
-  <si>
-    <t>violet</t>
-  </si>
-  <si>
-    <t>blanc</t>
-  </si>
-  <si>
-    <t>noir</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>A</t>
   </si>
@@ -41,38 +32,44 @@
     <t>B</t>
   </si>
   <si>
-    <t>A-1A</t>
-  </si>
-  <si>
-    <t>A-1B</t>
-  </si>
-  <si>
-    <t>B-1A</t>
-  </si>
-  <si>
-    <t>B-2A</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
     <t>D2</t>
   </si>
   <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D4</t>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>droite</t>
+  </si>
+  <si>
+    <t>gauche</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,9 +95,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H23"/>
+  <dimension ref="B1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,66 +400,40 @@
     <col min="8" max="8" width="5.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2</v>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -623,82 +597,86 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1">
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2">
         <v>0</v>
       </c>
     </row>
@@ -784,5 +762,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>